<commit_message>
Updated Selenium version, browsers, reports
</commit_message>
<xml_diff>
--- a/Maven_Hybrid_Framework/src/test/java/Test_Data/Login_IL.xlsx
+++ b/Maven_Hybrid_Framework/src/test/java/Test_Data/Login_IL.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8605DB-3A01-4226-A966-2A45A8E67726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CA7618-AFC4-4404-AA37-0CAAB3836805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -254,9 +254,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
     <t>chrome</t>
   </si>
   <si>
@@ -368,9 +365,6 @@
     <t>close browser</t>
   </si>
   <si>
-    <t>closeallbrowsers</t>
-  </si>
-  <si>
     <t>HFS</t>
   </si>
   <si>
@@ -414,6 +408,12 @@
   </si>
   <si>
     <t>TS21</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>closewindow</t>
   </si>
 </sst>
 </file>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -911,10 +911,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>6</v>
@@ -941,13 +941,13 @@
         <v>12</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -955,10 +955,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>13</v>
@@ -972,7 +972,7 @@
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -986,7 +986,7 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>16</v>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>20</v>
@@ -1038,10 +1038,10 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1049,7 +1049,9 @@
       <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="6"/>
+      <c r="J5" s="6" t="s">
+        <v>126</v>
+      </c>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
@@ -1059,7 +1061,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>23</v>
@@ -1084,19 +1086,19 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J7" s="6"/>
       <c r="L7" s="6"/>
@@ -1107,22 +1109,22 @@
         <v>3</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="G8" t="s">
-        <v>84</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="J8" s="6"/>
       <c r="L8" s="6"/>
@@ -1133,22 +1135,22 @@
         <v>3</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E9" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="G9" t="s">
-        <v>119</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>86</v>
       </c>
       <c r="J9" s="6"/>
       <c r="L9" s="6"/>
@@ -1161,7 +1163,7 @@
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>37</v>
@@ -1170,13 +1172,13 @@
         <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I10" t="s">
         <v>33</v>
@@ -1196,20 +1198,20 @@
         <v>40</v>
       </c>
       <c r="E11" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" t="s">
         <v>124</v>
       </c>
-      <c r="F11" t="s">
-        <v>126</v>
-      </c>
       <c r="G11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H11" t="s">
         <v>123</v>
-      </c>
-      <c r="H11" t="s">
-        <v>125</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
@@ -1225,16 +1227,16 @@
         <v>44</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" t="s">
         <v>124</v>
       </c>
-      <c r="F12" t="s">
-        <v>126</v>
-      </c>
       <c r="G12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -1248,7 +1250,7 @@
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>47</v>
@@ -1260,7 +1262,7 @@
         <v>32</v>
       </c>
       <c r="G13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" t="s">
         <v>59</v>
@@ -1281,7 +1283,7 @@
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>51</v>
@@ -1293,7 +1295,7 @@
         <v>32</v>
       </c>
       <c r="G14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H14" t="s">
         <v>60</v>
@@ -1313,7 +1315,7 @@
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>69</v>
@@ -1325,7 +1327,7 @@
         <v>32</v>
       </c>
       <c r="G15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H15" t="s">
         <v>61</v>
@@ -1347,7 +1349,7 @@
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>74</v>
@@ -1376,10 +1378,10 @@
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E17" t="s">
         <v>45</v>
@@ -1405,10 +1407,10 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E18" t="s">
         <v>45</v>
@@ -1433,13 +1435,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>110</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E19" t="s">
         <v>52</v>
@@ -1465,10 +1467,10 @@
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E20" t="s">
         <v>70</v>
@@ -1494,10 +1496,10 @@
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E21" t="s">
         <v>75</v>
@@ -1521,16 +1523,16 @@
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D22" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" t="s">
+        <v>114</v>
+      </c>
+      <c r="G22" t="s">
         <v>131</v>
-      </c>
-      <c r="E22" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" t="s">
-        <v>116</v>
       </c>
       <c r="J22" s="6"/>
       <c r="L22" s="6"/>
@@ -1618,8 +1620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1637,16 +1639,16 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>33</v>
@@ -1678,22 +1680,22 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
         <v>55</v>
@@ -1720,22 +1722,22 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G3" t="s">
         <v>55</v>
@@ -1762,22 +1764,19 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
+        <v>130</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G4" t="s">
         <v>55</v>
@@ -1798,7 +1797,7 @@
         <v>68</v>
       </c>
       <c r="M4" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="N4" s="8"/>
     </row>

</xml_diff>